<commit_message>
Added more content to tidyverse module
</commit_message>
<xml_diff>
--- a/data/nn_r_info_db.xlsx
+++ b/data/nn_r_info_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{80245BAD-4CBA-41A9-9FB1-77A78BB04A39}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{29B3B49C-9E14-4AE5-992E-2B87A13E5B12}"/>
   <bookViews>
-    <workbookView xWindow="14475" yWindow="300" windowWidth="18765" windowHeight="15300" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
+    <workbookView xWindow="16035" yWindow="300" windowWidth="14325" windowHeight="15300" activeTab="3" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
   <sheets>
     <sheet name="work_schedule" sheetId="1" r:id="rId1"/>
@@ -750,25 +750,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48762DA2-7B38-4373-94E1-F79287F51130}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.69921875" customWidth="1"/>
-    <col min="6" max="6" width="54.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" customWidth="1"/>
-    <col min="8" max="8" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.8984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="14.45" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -806,7 +806,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="27.95" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -880,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -938,7 +938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1221,43 +1221,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" ht="14.1" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
@@ -1274,11 +1274,11 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1380,12 +1380,12 @@
       <selection activeCell="A14" sqref="A14:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1408,7 +1408,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>9</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -1588,17 +1588,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C50C293-47F7-4CD9-B6F6-0CC1B0E1F86C}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.3984375" customWidth="1"/>
-    <col min="5" max="5" width="92.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="94.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="92.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="94.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1621,7 +1621,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1787,12 +1787,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1809,7 +1809,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>Shiny App Training</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>Shiny App Training</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6" t="e">
         <f>VLOOKUP($A6,books!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -1883,7 +1883,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" t="e">
         <f>VLOOKUP($A7,books!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -1893,7 +1893,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" t="e">
         <f>VLOOKUP($A8,books!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -1903,7 +1903,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="e">
         <f>VLOOKUP($A9,books!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -1913,7 +1913,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" t="e">
         <f>VLOOKUP($A10,books!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -1923,7 +1923,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11" t="e">
         <f>VLOOKUP($A11,books!$A:$B,2,FALSE)</f>
         <v>#N/A</v>
@@ -1944,7 +1944,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1960,6 +1960,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -2143,12 +2149,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
   <ds:schemaRefs>
@@ -2158,6 +2158,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2173,13 +2182,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated geospatial with recording
</commit_message>
<xml_diff>
--- a/data/nn_r_info_db.xlsx
+++ b/data/nn_r_info_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="454" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8E4F7FFF-FCBE-47A9-B596-3EA905C8FAE6}"/>
+  <xr:revisionPtr revIDLastSave="455" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{44F4FE51-4A1F-4BE8-8E01-28660CC9A59A}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="300" windowWidth="19080" windowHeight="15300" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
   <sheets>
     <sheet name="work_schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="112">
   <si>
     <t>week_start_date</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>https://web.microsoftstream.com/video/09c371d1-ecd8-4d08-b629-ba4a92839cf9</t>
+  </si>
+  <si>
+    <t>https://web.microsoftstream.com/video/d331753a-e974-4561-a00c-9145fb77bdb4</t>
   </si>
 </sst>
 </file>
@@ -1022,6 +1025,9 @@
       <c r="I8" s="7" t="s">
         <v>97</v>
       </c>
+      <c r="J8" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="K8">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A8)</f>
         <v>4</v>
@@ -1979,12 +1985,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -2168,6 +2168,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
   <ds:schemaRefs>
@@ -2177,15 +2183,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2201,4 +2198,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated with recording from Census module
</commit_message>
<xml_diff>
--- a/data/nn_r_info_db.xlsx
+++ b/data/nn_r_info_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="456" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{459F91A6-419A-41F2-BC63-B0E0103918EE}"/>
+  <xr:revisionPtr revIDLastSave="458" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{94CF9709-1F5E-4B1E-8C52-E297C01F4BE3}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="555" windowWidth="18840" windowHeight="15045" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
   <sheets>
     <sheet name="work_schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
   <si>
     <t>week_start_date</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>https://web.microsoftstream.com/embed/video/bad9e3fc-7693-4e17-ae4d-16c2d3bf9f1b</t>
+  </si>
+  <si>
+    <t>https://web.microsoftstream.com/video/5b33f7da-577d-4788-b5b4-0340340c41f4</t>
   </si>
 </sst>
 </file>
@@ -766,7 +769,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -780,7 +783,7 @@
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="72.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1105,6 +1108,9 @@
       </c>
       <c r="I10" s="7" t="s">
         <v>99</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="K10">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A10)</f>
@@ -1991,12 +1997,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -2180,6 +2180,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
   <ds:schemaRefs>
@@ -2189,15 +2195,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2213,4 +2210,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added recording link to table
</commit_message>
<xml_diff>
--- a/data/nn_r_info_db.xlsx
+++ b/data/nn_r_info_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="458" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{94CF9709-1F5E-4B1E-8C52-E297C01F4BE3}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{43D8D214-0FD2-43EC-AA6F-754462ECE877}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
   <si>
     <t>week_start_date</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>https://web.microsoftstream.com/video/5b33f7da-577d-4788-b5b4-0340340c41f4</t>
+  </si>
+  <si>
+    <t>https://web.microsoftstream.com/video/ba8007be-64a2-48a6-afe6-3da50cea5809</t>
   </si>
 </sst>
 </file>
@@ -769,7 +772,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1147,6 +1150,9 @@
       </c>
       <c r="I11" s="7" t="s">
         <v>100</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="K11">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A11)</f>
@@ -1997,6 +2003,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -2180,12 +2192,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
   <ds:schemaRefs>
@@ -2195,6 +2201,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2210,13 +2225,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added recording for GTFS
</commit_message>
<xml_diff>
--- a/data/nn_r_info_db.xlsx
+++ b/data/nn_r_info_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{43D8D214-0FD2-43EC-AA6F-754462ECE877}"/>
+  <xr:revisionPtr revIDLastSave="460" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{387AE58B-DCBF-44B9-92C0-B20CA67F3A2A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
+    <workbookView xWindow="14385" yWindow="60" windowWidth="23715" windowHeight="15405" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
   <sheets>
     <sheet name="work_schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="116">
   <si>
     <t>week_start_date</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>https://web.microsoftstream.com/video/ba8007be-64a2-48a6-afe6-3da50cea5809</t>
+  </si>
+  <si>
+    <t>https://web.microsoftstream.com/video/d0d59c49-a521-45e2-8dd0-58dbbf4626f8</t>
   </si>
 </sst>
 </file>
@@ -772,7 +775,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1189,6 +1192,9 @@
       </c>
       <c r="I12" s="7" t="s">
         <v>101</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="K12">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A12)</f>
@@ -2003,12 +2009,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -2192,6 +2192,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
   <ds:schemaRefs>
@@ -2201,15 +2207,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2225,4 +2222,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Drafted content for 10.13 lunch and learn
</commit_message>
<xml_diff>
--- a/data/nn_r_info_db.xlsx
+++ b/data/nn_r_info_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="460" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{387AE58B-DCBF-44B9-92C0-B20CA67F3A2A}"/>
+  <xr:revisionPtr revIDLastSave="461" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8DDB7874-9EA3-4C56-9982-1B034A0EA448}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="60" windowWidth="23715" windowHeight="15405" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
+    <workbookView xWindow="17700" yWindow="0" windowWidth="11115" windowHeight="12360" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
   <sheets>
     <sheet name="work_schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
   <si>
     <t>week_start_date</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>https://web.microsoftstream.com/video/d0d59c49-a521-45e2-8dd0-58dbbf4626f8</t>
+  </si>
+  <si>
+    <t>https://web.microsoftstream.com/video/a0ef1f1d-fec8-47c9-b7da-17466d82e21a</t>
   </si>
 </sst>
 </file>
@@ -774,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48762DA2-7B38-4373-94E1-F79287F51130}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -1231,6 +1234,9 @@
       </c>
       <c r="I13" s="7" t="s">
         <v>102</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="K13">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A13)</f>
@@ -2009,6 +2015,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -2192,12 +2204,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
   <ds:schemaRefs>
@@ -2207,6 +2213,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2222,13 +2237,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added recording for misc. questions session
</commit_message>
<xml_diff>
--- a/data/nn_r_info_db.xlsx
+++ b/data/nn_r_info_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/bblanc_nelsonnygaard_com/Documents/Documents/Internal/R Training/nn_r_training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="461" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8DDB7874-9EA3-4C56-9982-1B034A0EA448}"/>
+  <xr:revisionPtr revIDLastSave="463" documentId="8_{6EEC280C-549B-4236-9B18-788A18C57CBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{100AC1DA-687B-4C78-B8A2-E0B834DB8699}"/>
   <bookViews>
-    <workbookView xWindow="17700" yWindow="0" windowWidth="11115" windowHeight="12360" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B62E98FC-35F5-4677-B9D8-11BC7E79779C}"/>
   </bookViews>
   <sheets>
     <sheet name="work_schedule" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>week_start_date</t>
   </si>
@@ -349,9 +349,6 @@
     <t>topics_output/shiny_4.html</t>
   </si>
   <si>
-    <t>topics_output/rmarkdown.html</t>
-  </si>
-  <si>
     <t>topics_output/tidyverse.html</t>
   </si>
   <si>
@@ -389,6 +386,12 @@
   </si>
   <si>
     <t>https://web.microsoftstream.com/video/a0ef1f1d-fec8-47c9-b7da-17466d82e21a</t>
+  </si>
+  <si>
+    <t>topic_output/misc_questions.html</t>
+  </si>
+  <si>
+    <t>https://web.microsoftstream.com/video/f3b1ef12-798f-45fd-b75a-ddd3dd295fc8</t>
   </si>
 </sst>
 </file>
@@ -777,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48762DA2-7B38-4373-94E1-F79287F51130}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -810,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -825,7 +828,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>58</v>
@@ -950,7 +953,7 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -962,10 +965,10 @@
         <v>0.5</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K6">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A6)</f>
@@ -988,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -1003,7 +1006,7 @@
         <v>96</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K7">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A7)</f>
@@ -1026,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1041,7 +1044,7 @@
         <v>97</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K8">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A8)</f>
@@ -1064,7 +1067,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -1080,7 +1083,7 @@
         <v>98</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K9">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A9)</f>
@@ -1103,7 +1106,7 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1119,7 +1122,7 @@
         <v>99</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K10">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A10)</f>
@@ -1142,7 +1145,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -1158,7 +1161,7 @@
         <v>100</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K11">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A11)</f>
@@ -1181,7 +1184,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
         <v>18</v>
@@ -1197,7 +1200,7 @@
         <v>101</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K12">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A12)</f>
@@ -1220,7 +1223,7 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -1236,7 +1239,7 @@
         <v>102</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K13">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A13)</f>
@@ -1257,7 +1260,7 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -1269,7 +1272,10 @@
         <v>0.5</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>103</v>
+        <v>116</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="K14">
         <f>SUMIFS(datacamp_courses!$E:$E,datacamp_courses!$A:$A,work_schedule!A14)</f>
@@ -2015,12 +2021,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010030D8ABC80AF248409B062131ADAEB348" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f2c104d79b850790102affc578e3f3df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7a9084b5-aaea-4044-97e5-7df1b6c14389" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c945aebc172d2c3def17dd61454be78a" ns3:_="">
     <xsd:import namespace="7a9084b5-aaea-4044-97e5-7df1b6c14389"/>
@@ -2204,6 +2204,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E47575C-B9BF-447D-9E40-B23BD982C7E2}">
   <ds:schemaRefs>
@@ -2213,15 +2219,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B41D2027-88CA-4472-8A36-B9A2BF4C21CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2237,4 +2234,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F49FA1FB-4E38-4DBA-AA91-8BC5AEAA708C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>